<commit_message>
This is my branch 05062022
</commit_message>
<xml_diff>
--- a/bin/Debug/Output/05062022/For Out as of 05062022.xlsx
+++ b/bin/Debug/Output/05062022/For Out as of 05062022.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Order ID</t>
   </si>
@@ -270,6 +270,12 @@
   </si>
   <si>
     <t>5/6/2022 3:50:33 AM</t>
+  </si>
+  <si>
+    <t>2203271DY8MNV3</t>
+  </si>
+  <si>
+    <t>5/6/2022 4:24:05 AM</t>
   </si>
 </sst>
 </file>
@@ -315,7 +321,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1321,6 +1327,106 @@
         <v>85</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>